<commit_message>
new version for sales credit calc
</commit_message>
<xml_diff>
--- a/SalesCredit_Model_License_v1_cvs.xlsx
+++ b/SalesCredit_Model_License_v1_cvs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cvs/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cvs/Documents/GitHub/moontshot/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -40,6 +40,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Christian von Stengel:</t>
         </r>
@@ -48,6 +49,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 enter new license target for this fy</t>
@@ -62,6 +64,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Christian von Stengel:</t>
         </r>
@@ -70,6 +73,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 enter license target with existing clients</t>
@@ -84,6 +88,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Christian von Stengel:</t>
         </r>
@@ -92,6 +97,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 enter value to weigh new logo license in regards to existing clients</t>
@@ -106,6 +112,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Christian von Stengel:</t>
         </r>
@@ -114,6 +121,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 einter weight for exisitng clients license revenue. Will be "1" in most cases</t>
@@ -128,6 +136,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Christian von Stengel:</t>
         </r>
@@ -136,6 +145,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 enter overassignment for sales reps in % of taeget</t>
@@ -150,6 +160,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Christian von Stengel:</t>
         </r>
@@ -158,6 +169,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Rep target in sales credits</t>
@@ -172,6 +184,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Christian von Stengel:</t>
         </r>
@@ -180,6 +193,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Sales Credits per USD license revenue with new logos</t>
@@ -194,6 +208,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Christian von Stengel:</t>
         </r>
@@ -202,6 +217,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Sales Credits per license USD for existing clients</t>
@@ -312,12 +328,14 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -692,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,19 +795,19 @@
         <v>18</v>
       </c>
       <c r="D7" s="7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E7" s="2">
         <f>E3*(1+D7)</f>
-        <v>5500000</v>
+        <v>6000000</v>
       </c>
       <c r="F7" s="22">
         <f>E7*F4</f>
-        <v>3300000</v>
+        <v>3600000</v>
       </c>
       <c r="G7" s="22">
         <f>E7*G4</f>
-        <v>2200000</v>
+        <v>2400000</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
@@ -848,7 +866,7 @@
       </c>
       <c r="F15" s="2">
         <f>E17*F7</f>
-        <v>3599999.9999999995</v>
+        <v>3600000</v>
       </c>
       <c r="G15" s="2">
         <f>E17*G7</f>
@@ -891,15 +909,15 @@
       <c r="D17" s="16"/>
       <c r="E17" s="19">
         <f>E15/E7</f>
-        <v>1.0909090909090908</v>
+        <v>1</v>
       </c>
       <c r="F17" s="23">
         <f>G17*F5</f>
-        <v>1.3636363636363635</v>
+        <v>1.25</v>
       </c>
       <c r="G17" s="23">
         <f>E17/(F5*F4+G5*G4)</f>
-        <v>0.68181818181818177</v>
+        <v>0.625</v>
       </c>
       <c r="H17" s="4">
         <f>E17-(F17*F4+G17*G4)</f>

</xml_diff>